<commit_message>
TextInputScreen implemented for gathering data during character gen.
</commit_message>
<xml_diff>
--- a/data/character_creation.xlsx
+++ b/data/character_creation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="18540" yWindow="6060" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>main_title</t>
   </si>
@@ -38,12 +38,6 @@
     <t>card_image</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
     <t>Character Gender</t>
   </si>
   <si>
@@ -77,12 +71,6 @@
     <t>card_type</t>
   </si>
   <si>
-    <t>CharacterCard</t>
-  </si>
-  <si>
-    <t>TextInput</t>
-  </si>
-  <si>
     <t>Character First Name</t>
   </si>
   <si>
@@ -144,6 +132,12 @@
   </si>
   <si>
     <t>portrait</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>TextInputScreen</t>
   </si>
 </sst>
 </file>
@@ -458,82 +452,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" customWidth="1"/>
-    <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -541,132 +527,96 @@
       <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E7" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>